<commit_message>
auto y eva finalizado y por finalizar
</commit_message>
<xml_diff>
--- a/Formato envio correos_.xlsx
+++ b/Formato envio correos_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCP Effio\Documents\Envio-auto-de-correos-outlook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFFD49B-016F-4733-AA0D-BA1A3429B4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDFCEBD-2642-4AED-A9CA-2EEB672AF5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE!$A$1:$E$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE!$A$1:$E$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="107">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -56,9 +56,6 @@
     <t>dserrano@bcp.com.pe</t>
   </si>
   <si>
-    <t>rplaz@bcp.com.pe</t>
-  </si>
-  <si>
     <t>schavezr@bcp.com.pe</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>jpoquioma@bcp.com.pe</t>
   </si>
   <si>
-    <t>jvillegas@bcp.com.pe</t>
-  </si>
-  <si>
     <t>carlosgutierrezr@bcp.com.pe</t>
   </si>
   <si>
@@ -101,69 +95,33 @@
     <t>jorgemayorga@bcp.com.pe</t>
   </si>
   <si>
-    <t>victoryomona@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>jaimemunoz@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>jorgechavezm@bcp.com.pe</t>
-  </si>
-  <si>
     <t>jordinymontanez@bcp.com.pe</t>
   </si>
   <si>
-    <t>heliamordejoiti@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>joseventura@bcp.com.pe</t>
-  </si>
-  <si>
     <t>edwinmunoz@bcp.com.pe</t>
   </si>
   <si>
-    <t>ginoreyna@bcp.com.pe</t>
-  </si>
-  <si>
     <t>washingtonquerol@bcp.com.pe</t>
   </si>
   <si>
     <t>eduardosausurin@bcp.com.pe</t>
   </si>
   <si>
-    <t>edgarsalamanca@bcp.com.pe</t>
-  </si>
-  <si>
-    <t>juanorjuela@bcp.com.pe</t>
-  </si>
-  <si>
     <t>tomasgonzalez@bcp.com.pe</t>
   </si>
   <si>
-    <t>jesusmunera@bcp.com.pe</t>
-  </si>
-  <si>
     <t>edgardalva@bcp.com.pe</t>
   </si>
   <si>
     <t>ivangarcia@bcp.com.pe</t>
   </si>
   <si>
-    <t>ellanos@bcp.com.pe</t>
-  </si>
-  <si>
     <t>calderete@bcp.com.pe</t>
   </si>
   <si>
     <t>T27125</t>
   </si>
   <si>
-    <t>T28469</t>
-  </si>
-  <si>
-    <t>T27115</t>
-  </si>
-  <si>
     <t>T28462</t>
   </si>
   <si>
@@ -176,9 +134,6 @@
     <t>E16891</t>
   </si>
   <si>
-    <t>S00347</t>
-  </si>
-  <si>
     <t>S00823</t>
   </si>
   <si>
@@ -191,9 +146,6 @@
     <t>S62040</t>
   </si>
   <si>
-    <t>S71114</t>
-  </si>
-  <si>
     <t>S92895</t>
   </si>
   <si>
@@ -221,263 +173,197 @@
     <t>T17438</t>
   </si>
   <si>
-    <t>T17676</t>
-  </si>
-  <si>
-    <t>T18500</t>
-  </si>
-  <si>
-    <t>T18525</t>
-  </si>
-  <si>
     <t>T19788</t>
   </si>
   <si>
-    <t>T19796</t>
-  </si>
-  <si>
-    <t>T22925</t>
-  </si>
-  <si>
     <t>T24467</t>
   </si>
   <si>
-    <t>T29902</t>
-  </si>
-  <si>
     <t>T30402</t>
   </si>
   <si>
-    <t>T30405</t>
-  </si>
-  <si>
     <t>T30864</t>
   </si>
   <si>
     <t>T31403</t>
   </si>
   <si>
-    <t>U17256</t>
-  </si>
-  <si>
     <t>U21691</t>
   </si>
   <si>
     <t>EMAIL_CAL</t>
   </si>
   <si>
-    <t>Jefferson Francisco Santos Centeno, Luis Alfonso Quispe Aylas</t>
-  </si>
-  <si>
     <t>Joseph Campos Gilvonio</t>
   </si>
   <si>
-    <t>Maryl Carolina Abanto Herrera</t>
-  </si>
-  <si>
     <t>Sandy Paola Troncos Valencia</t>
   </si>
   <si>
-    <t>Cesar Maicohol Olivares Leona, Hans Richard Villaizan Yamamoto, Wilcos Jhon Condor Pucuhuayla, Wilmar Rafael Muñoz Bravo</t>
-  </si>
-  <si>
     <t>Junior Mariano Carrión Rodríguez</t>
   </si>
   <si>
-    <t>Jose Alonso Rosas Gamarra, Juan Manuel Vasquez Fonseca</t>
-  </si>
-  <si>
-    <t>Luis Rodolfo Perez Soriano</t>
-  </si>
-  <si>
     <t>Diego David Bermudez Rodriguez</t>
   </si>
   <si>
-    <t>Julio Nicolas Juarez Moran, Renny Donny Rodriguez Espinoza, Richar Marvin Fernández Vilchez</t>
-  </si>
-  <si>
     <t>Diego Alonso Reyes Molina</t>
   </si>
   <si>
     <t>Eloy Ivan Solano Coello</t>
   </si>
   <si>
-    <t>Eloy Eduardo Santillan Caballero, Gonzalo Emilio Salas Seguel, Pedro Rafael Bedoya Marrugo</t>
-  </si>
-  <si>
-    <t>Marcos Enrique Morales Angulo, Romer Angel Vargas Otiniano</t>
-  </si>
-  <si>
-    <t>Edgar Mauricio Salamanca Pedraza, Washington Junior Querol De La Serna</t>
-  </si>
-  <si>
-    <t>Edwin Jhon Vásquez Mondragón, Evelyn Daniela Sariego Rivera, Giancarlo Renato Palomino Huallpa</t>
-  </si>
-  <si>
-    <t>Gino Reyna Bellido, Luis Fernando Chavez Lucich, Raul Gustavo Pacheco Nuñez</t>
-  </si>
-  <si>
-    <t>Cesar Augusto Prado Vasquez</t>
-  </si>
-  <si>
-    <t>Carlos Andres Santacruz Zambrano</t>
-  </si>
-  <si>
-    <t>Raúl Joseph Aguirre Moisés</t>
-  </si>
-  <si>
     <t>Andre Robinson Yataco Lermo</t>
   </si>
   <si>
-    <t>Ignacio Margallo Nn, Jhon Jairo Muñoz Mateus</t>
-  </si>
-  <si>
-    <t>Jhon Wilder Lozano Tapia</t>
-  </si>
-  <si>
-    <t>Arnold Raúl Matias De La Cruz, Petter Jack Alva Gazani</t>
-  </si>
-  <si>
-    <t>Guadalupe Carranza Villa, Rodol Harry Coa Limasca</t>
-  </si>
-  <si>
-    <t>Giancarlo Alejandro Manzano Juárez, Gustavo Adolfo Vielma Anaya</t>
-  </si>
-  <si>
-    <t>Carlos Augusto Nole Machaca</t>
-  </si>
-  <si>
-    <t>Yeisson Kevin Vivar Rodriguez</t>
-  </si>
-  <si>
     <t>Christian Italo Espinoza Ochoa</t>
   </si>
   <si>
-    <t>Ronald Ramón Pareja Alcazaba, Steffy Ivonne Luna Carrion</t>
-  </si>
-  <si>
     <t>Frans Juan Valdivia Chavez</t>
   </si>
   <si>
     <t>Gustavo Elmer Meza Nuñez</t>
   </si>
   <si>
-    <t>Bryan King Atoche, Jose Francisco Valdez Nn, Juan Carlos Fernandez Baldeon</t>
-  </si>
-  <si>
-    <t>Anggelo Marccelo Urso Goddard, Daniel Hernando Olarte Bohorquez, Eduardo Sausurin Nn</t>
-  </si>
-  <si>
-    <t>Carlos Enrique Muñoz Galvez</t>
-  </si>
-  <si>
-    <t>Diana Julissa Serrano Ramirez</t>
-  </si>
-  <si>
-    <t>Rene Ruben Plaz Cabrera</t>
-  </si>
-  <si>
-    <t>Silvana Jeannette Chavez Rios</t>
-  </si>
-  <si>
-    <t>Pedro Manuel Varillas Obregon</t>
-  </si>
-  <si>
-    <t>Fernando Pierino Gomez Jaime</t>
-  </si>
-  <si>
-    <t>Jeysson Marcial Poquioma Huaman</t>
-  </si>
-  <si>
-    <t>Javier Enrique Villegas Herrera</t>
-  </si>
-  <si>
-    <t>Carlos Aquiles Gutierrez Ronceros</t>
-  </si>
-  <si>
-    <t>Jhon Anthony Alvarez Borja</t>
-  </si>
-  <si>
-    <t>Franklin Arturo Romero Mejia</t>
-  </si>
-  <si>
-    <t>Danilo Nicolas Mendoza Ricaldi</t>
-  </si>
-  <si>
-    <t>Christian Martín Ramos Vega</t>
-  </si>
-  <si>
-    <t>Jonathan Choy Rivera</t>
-  </si>
-  <si>
-    <t>Renzo Omar Sánchez Pezo</t>
-  </si>
-  <si>
-    <t>Daniella Anddrea Rojas Pacheco</t>
-  </si>
-  <si>
-    <t>Jorge Mayorga Martinez</t>
-  </si>
-  <si>
-    <t>Victor Jaiden Yomona Aguilar</t>
-  </si>
-  <si>
-    <t>Jaime Alfredo Muñoz Perez</t>
-  </si>
-  <si>
-    <t>Jorge Chavez Mondragon</t>
-  </si>
-  <si>
-    <t>Jordiny Montañez Flores</t>
-  </si>
-  <si>
-    <t>Heliam Jose Ordejoiti Sojo</t>
-  </si>
-  <si>
-    <t>Jose Santos Ventura Arteaga</t>
-  </si>
-  <si>
-    <t>Edwin Humberto Muñoz Ramirez</t>
-  </si>
-  <si>
-    <t>Gino Reyna Bellido</t>
-  </si>
-  <si>
-    <t>Washington Junior Querol De La Serna</t>
-  </si>
-  <si>
-    <t>Eduardo Sausurin Nn</t>
-  </si>
-  <si>
-    <t>Edgar Mauricio Salamanca Pedraza</t>
-  </si>
-  <si>
-    <t>Juan Jose Orjuela Castillo</t>
-  </si>
-  <si>
-    <t>Tomás Alejandro González Cáceres</t>
-  </si>
-  <si>
-    <t>Jesus David Munera Alvarez</t>
-  </si>
-  <si>
-    <t>Edgard Alva Fajardo</t>
-  </si>
-  <si>
-    <t>Ivan Venor Garcia Baños</t>
-  </si>
-  <si>
-    <t>Eric Miguel Llanos Palomino</t>
-  </si>
-  <si>
-    <t>Carmela Rosario Alderete Campos</t>
+    <t>T06901</t>
+  </si>
+  <si>
+    <t>victormespinoza@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Silvana</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Jeysson</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Danilo</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Renzo</t>
+  </si>
+  <si>
+    <t>Daniella</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Jordiny</t>
+  </si>
+  <si>
+    <t>Edwin</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Tomás</t>
+  </si>
+  <si>
+    <t>Edgard</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Carmela</t>
+  </si>
+  <si>
+    <t>Luis Alfonso Quispe Aylas // Jefferson Francisco Santos Centeno</t>
+  </si>
+  <si>
+    <t>Wilcos Jhon Condor Pucuhuayla // Wilmar Rafael Muñoz Bravo</t>
+  </si>
+  <si>
+    <t>Juan Manuel Vasquez Fonseca // Jose Alonso Rosas Gamarra</t>
+  </si>
+  <si>
+    <t>Julio Nicolas Juarez Moran // Renny Donny Rodriguez Espinoza // Richar Marvin Fernández Vilchez</t>
+  </si>
+  <si>
+    <t>Eloy Eduardo Santillan Caballero // Pedro Rafael Bedoya Marrugo // Gonzalo Emilio Salas Seguel</t>
+  </si>
+  <si>
+    <t>Marcos Enrique Morales Angulo</t>
+  </si>
+  <si>
+    <t>Marco Boris Maquera Quispe</t>
+  </si>
+  <si>
+    <t>Washington Junior Querol De La Serna // Edgar Mauricio Salamanca Pedraza</t>
+  </si>
+  <si>
+    <t>Evelyn Daniela Sariego Rivera // Edwin Jhon Vásquez Mondragón // Giancarlo Renato Palomino Huallpa</t>
+  </si>
+  <si>
+    <t>Luis Fernando Chavez Lucich // Raul Gustavo Pacheco Nuñez // Gino Reyna Bellido</t>
+  </si>
+  <si>
+    <t>Rodol Harry Coa Limasca // Guadalupe Carranza Villa</t>
+  </si>
+  <si>
+    <t>Gustavo Adolfo Vielma Anaya // Giancarlo Alejandro Manzano Juárez</t>
+  </si>
+  <si>
+    <t>Eduardo Sausurin Nn // Daniel Hernando Olarte Bohorquez // Anggelo Marccelo Urso Goddard</t>
+  </si>
+  <si>
+    <t>mbravo@bcp.com.pe; valeriaroman@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>daniellarojas@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>renzoosanchez@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>carlosmunozg@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>calderete@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>joelretuertoo@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
+  </si>
+  <si>
+    <t>tomasgonzalez@bcp.com.pe; valeriaroman@bcp.com.pe; mbravo@bcp.com.pe; jmazuelos@bcp.com.pe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,13 +500,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -967,17 +846,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1333,19 +1203,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="115" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1359,7 +1229,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1367,500 +1237,413 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>76</v>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>77</v>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>78</v>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>79</v>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>80</v>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>81</v>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>82</v>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>83</v>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>84</v>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>85</v>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>86</v>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>87</v>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>89</v>
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>91</v>
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>93</v>
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>94</v>
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>95</v>
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>96</v>
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>97</v>
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>98</v>
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E36" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>